<commit_message>
updated appium tests with updated locators
</commit_message>
<xml_diff>
--- a/testdata/MobileTestData.xlsx
+++ b/testdata/MobileTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angee/EclipseProjects/XOME/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1674D569-CD49-AF49-A5F6-313D979C716E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6893C991-9394-744D-AC02-1837B5AB7461}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="6520" windowWidth="28040" windowHeight="7400" firstSheet="9" activeTab="18" xr2:uid="{76F26415-F998-4140-9827-0198A1E793B3}"/>
+    <workbookView xWindow="4740" yWindow="6640" windowWidth="24840" windowHeight="8600" firstSheet="11" activeTab="18" xr2:uid="{76F26415-F998-4140-9827-0198A1E793B3}"/>
   </bookViews>
   <sheets>
     <sheet name="mSortByLowtoHighPrice" sheetId="1" r:id="rId1"/>
@@ -745,7 +745,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>